<commit_message>
Updated tables with ANOVA results
</commit_message>
<xml_diff>
--- a/analyses/tables/allometry.xlsx
+++ b/analyses/tables/allometry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicksmith/Documents/Git/mdi_pitchpine/analyses/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/risa/Desktop/work/Smith Lab/mdi_pitchpine-master/analyses/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C6AFE78A-3B6B-7C46-97E0-3826331CB162}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD70EC7C-CEA6-894F-B251-1D812E9A1288}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10480" yWindow="5120" windowWidth="26440" windowHeight="15440"/>
+    <workbookView xWindow="6220" yWindow="7680" windowWidth="26440" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allometry" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Df</t>
   </si>
@@ -51,11 +51,14 @@
   <si>
     <t>Tree Height</t>
   </si>
+  <si>
+    <t>Density</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -558,10 +561,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -916,11 +921,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -935,7 +940,7 @@
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -950,8 +955,12 @@
         <v>8</v>
       </c>
       <c r="H1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -974,8 +983,14 @@
       <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1000,8 +1015,14 @@
       <c r="H3" s="2">
         <v>3.0624167867085001E-3</v>
       </c>
+      <c r="I3" s="1">
+        <v>9.9256566903657202</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2.61584470605467E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1026,8 +1047,14 @@
       <c r="H4" s="2">
         <v>7.2674724865066806E-2</v>
       </c>
+      <c r="I4" s="1">
+        <v>1.4811933245348901</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.228692100700884</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1052,8 +1079,14 @@
       <c r="H5" s="2">
         <v>1.8482563349575602E-2</v>
       </c>
+      <c r="I5" s="1">
+        <v>9.4292807271495697E-3</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.92299012646156697</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1066,6 +1099,12 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updates to analysis & docs
</commit_message>
<xml_diff>
--- a/analyses/tables/allometry.xlsx
+++ b/analyses/tables/allometry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/risa/Desktop/work/Smith Lab/mdi_pitchpine-master/analyses/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/risa/Git/mdi_pitchpine/analyses/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD70EC7C-CEA6-894F-B251-1D812E9A1288}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684245CD-5400-0041-9403-9D8A9FFBCF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6220" yWindow="7680" windowWidth="26440" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2360" yWindow="500" windowWidth="26440" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allometry" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
-  <si>
-    <t>Df</t>
-  </si>
-  <si>
-    <t>Residuals</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>Elevation</t>
   </si>
@@ -34,25 +28,34 @@
     <t>Fire</t>
   </si>
   <si>
-    <t>Elevation*Fire</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
-    <t>Canopy Spread</t>
+    <t>Chisq</t>
   </si>
   <si>
-    <t>DBH</t>
+    <t>Elevation:Fire</t>
   </si>
   <si>
-    <t>Tree Height</t>
+    <t>Tree Height (m)</t>
   </si>
   <si>
-    <t>Density</t>
+    <t>Canopy Spread (m)</t>
+  </si>
+  <si>
+    <t>DBH (cm)</t>
+  </si>
+  <si>
+    <t>Distance Between Neighbors (m)</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>Pr(&gt;Chisq)</t>
+  </si>
+  <si>
+    <t>Slope</t>
   </si>
 </sst>
 </file>
@@ -386,7 +389,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -501,21 +504,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -561,12 +549,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -922,177 +911,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C3" sqref="C3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1"/>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>6</v>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1.47821059364559</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.224054701517613</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3.4506568866817</v>
+      </c>
+      <c r="F3" s="4">
+        <v>6.3226636985205503E-2</v>
+      </c>
+      <c r="G3" s="4">
+        <v>7.9478606241921304</v>
+      </c>
+      <c r="H3" s="4">
+        <v>4.8144255879687802E-3</v>
+      </c>
+      <c r="I3" s="4">
+        <v>3.4334037040636098</v>
+      </c>
+      <c r="J3" s="4">
+        <v>6.3890299103552095E-2</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0.68329848469389598</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0.40845321160451398</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
-        <v>2.2201069545966701</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.14493367296637799</v>
-      </c>
-      <c r="E3" s="2">
-        <v>8.3352229839036198</v>
-      </c>
-      <c r="F3" s="2">
-        <v>6.53768196518592E-3</v>
-      </c>
-      <c r="G3" s="2">
-        <v>10.083847188342601</v>
-      </c>
-      <c r="H3" s="2">
-        <v>3.0624167867085001E-3</v>
-      </c>
-      <c r="I3" s="1">
-        <v>9.9256566903657202</v>
-      </c>
-      <c r="J3" s="1">
-        <v>2.61584470605467E-3</v>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1.54169292873015</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.21436599192908801</v>
+      </c>
+      <c r="E4" s="4">
+        <v>9.7244709218031106E-2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.75516148506394998</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1.18694766411483E-2</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.91324442655978599</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.15696794685294199</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.69196353593496096</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1.2403247674536599E-2</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0.91132305261490199</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
-        <v>0.511581785196213</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.47906826376046402</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.241640476362215</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.62600770642063996</v>
-      </c>
-      <c r="G4" s="2">
-        <v>3.4190109693101798</v>
-      </c>
-      <c r="H4" s="2">
-        <v>7.2674724865066806E-2</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1.4811933245348901</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0.228692100700884</v>
+      <c r="C5" s="5">
+        <v>0.25986113488504198</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.61021557302515705</v>
+      </c>
+      <c r="E5" s="4">
+        <v>6.5933298460407999</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1.02361536447687E-2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>6.83577066836384E-2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.79374313748962599</v>
+      </c>
+      <c r="I5" s="4">
+        <v>6.0566437819975803E-2</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.805602892091001</v>
+      </c>
+      <c r="K5" s="4">
+        <v>2.9296309354558301</v>
+      </c>
+      <c r="L5" s="4">
+        <v>8.6967371356631296E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
-        <v>8.0627873898582294</v>
-      </c>
-      <c r="D5" s="2">
-        <v>7.38505461824985E-3</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.42017868455690699</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.52096121333617096</v>
-      </c>
-      <c r="G5" s="2">
-        <v>6.0899005409589702</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1.8482563349575602E-2</v>
-      </c>
-      <c r="I5" s="1">
-        <v>9.4292807271495697E-3</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0.92299012646156697</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1">
-        <v>36</v>
-      </c>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1101,10 +1116,22 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
switched back to linear models and made relevant changes
</commit_message>
<xml_diff>
--- a/analyses/tables/allometry.xlsx
+++ b/analyses/tables/allometry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/risa/Git/mdi_pitchpine/analyses/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684245CD-5400-0041-9403-9D8A9FFBCF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CC9588-6841-374B-9F97-FB0582897224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="500" windowWidth="26440" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2840" yWindow="8280" windowWidth="26440" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allometry" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>Elevation</t>
   </si>
@@ -28,16 +28,7 @@
     <t>Fire</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Chisq</t>
-  </si>
-  <si>
     <t>Elevation:Fire</t>
-  </si>
-  <si>
-    <t>Tree Height (m)</t>
   </si>
   <si>
     <t>Canopy Spread (m)</t>
@@ -49,13 +40,19 @@
     <t>Distance Between Neighbors (m)</t>
   </si>
   <si>
-    <t>df</t>
+    <t>Slope</t>
   </si>
   <si>
-    <t>Pr(&gt;Chisq)</t>
+    <t>Df</t>
   </si>
   <si>
-    <t>Slope</t>
+    <t>F value</t>
+  </si>
+  <si>
+    <t>Pr(&gt;F)</t>
+  </si>
+  <si>
+    <t>Tree Height</t>
   </si>
 </sst>
 </file>
@@ -549,12 +546,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -911,215 +907,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="N1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3"/>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1.47821059364559</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0.224054701517613</v>
-      </c>
-      <c r="E3" s="4">
-        <v>3.4506568866817</v>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>8.1736406729407705</v>
+      </c>
+      <c r="D3" s="4">
+        <v>7.0268487106686E-3</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
       <c r="F3" s="4">
-        <v>6.3226636985205503E-2</v>
+        <v>16.080211224543898</v>
       </c>
       <c r="G3" s="4">
-        <v>7.9478606241921304</v>
-      </c>
-      <c r="H3" s="4">
-        <v>4.8144255879687802E-3</v>
+        <v>2.9279753968443697E-4</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
       </c>
       <c r="I3" s="4">
-        <v>3.4334037040636098</v>
+        <v>19.763689122637199</v>
       </c>
       <c r="J3" s="4">
-        <v>6.3890299103552095E-2</v>
-      </c>
-      <c r="K3" s="4">
-        <v>0.68329848469389598</v>
+        <v>2.483241139549E-4</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
       </c>
       <c r="L3" s="4">
-        <v>0.40845321160451398</v>
+        <v>21.5770494047526</v>
+      </c>
+      <c r="M3" s="4">
+        <v>2.10294935854568E-5</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" s="4">
+        <v>3.8623532293126499</v>
+      </c>
+      <c r="P3" s="4">
+        <v>5.7132906292297697E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1.54169292873015</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.21436599192908801</v>
-      </c>
-      <c r="E4" s="4">
-        <v>9.7244709218031106E-2</v>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.18694766411424E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.91384944121357004</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
       <c r="F4" s="4">
-        <v>0.75516148506394998</v>
+        <v>1.10000951507023</v>
       </c>
       <c r="G4" s="4">
-        <v>1.18694766411483E-2</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0.91324442655978599</v>
+        <v>0.30125445137128398</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
       </c>
       <c r="I4" s="4">
-        <v>0.15696794685294199</v>
+        <v>1.4181998517729</v>
       </c>
       <c r="J4" s="4">
-        <v>0.69196353593496096</v>
-      </c>
-      <c r="K4" s="4">
-        <v>1.2403247674536599E-2</v>
+        <v>0.24764252610956899</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
       </c>
       <c r="L4" s="4">
-        <v>0.91132305261490199</v>
+        <v>113.804564131031</v>
+      </c>
+      <c r="M4" s="4">
+        <v>4.1674708884916503E-15</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4" s="4">
+        <v>9.7244709217943398E-2</v>
+      </c>
+      <c r="P4" s="4">
+        <v>0.75696043995184303</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0.25986113488504198</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0.61021557302515705</v>
-      </c>
-      <c r="E5" s="4">
-        <v>6.5933298460407999</v>
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>6.8357706683642702E-2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.79523320122453001</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
       </c>
       <c r="F5" s="4">
-        <v>1.02361536447687E-2</v>
+        <v>3.0218002883814399</v>
       </c>
       <c r="G5" s="4">
-        <v>6.83577066836384E-2</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0.79374313748962599</v>
+        <v>9.0699818525649206E-2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
       </c>
       <c r="I5" s="4">
-        <v>6.0566437819975803E-2</v>
+        <v>0.467852370292895</v>
       </c>
       <c r="J5" s="4">
-        <v>0.805602892091001</v>
-      </c>
-      <c r="K5" s="4">
-        <v>2.9296309354558301</v>
+        <v>0.50182596240097299</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
       </c>
       <c r="L5" s="4">
-        <v>8.6967371356631296E-2</v>
+        <v>108.085425093246</v>
+      </c>
+      <c r="M5" s="4">
+        <v>1.0966392463473E-14</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4">
+        <v>6.5933298460407901</v>
+      </c>
+      <c r="P5" s="4">
+        <v>1.4533845522818001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="B6">
+        <v>36</v>
+      </c>
+      <c r="E6">
+        <v>36</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+      <c r="K6">
+        <v>56</v>
+      </c>
+      <c r="N6">
+        <v>36</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>

</xml_diff>

<commit_message>
final updates before shipping back to jeff
</commit_message>
<xml_diff>
--- a/analyses/tables/allometry.xlsx
+++ b/analyses/tables/allometry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/risa/Git/mdi_pitchpine/analyses/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicksmith/Documents/Git/mdi_pitchpine/analyses/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CC9588-6841-374B-9F97-FB0582897224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CFA90F-81DA-5149-9BC3-9A43D0D1C628}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="8280" windowWidth="26440" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10960" yWindow="6160" windowWidth="26440" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allometry" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
   <si>
     <t>Elevation</t>
   </si>
@@ -54,6 +54,9 @@
   <si>
     <t>Tree Height</t>
   </si>
+  <si>
+    <t>&lt;0.001</t>
+  </si>
 </sst>
 </file>
 
@@ -62,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,9 +203,22 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -546,12 +562,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -910,283 +928,292 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B3" sqref="B3:P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="N1" s="3" t="s">
+      <c r="L1" s="1"/>
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4">
-        <v>8.1736406729407705</v>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>7.9478606241921899</v>
       </c>
       <c r="D3" s="4">
-        <v>7.0268487106686E-3</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4">
-        <v>16.080211224543898</v>
+        <v>7.7771897558913403E-3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>13.7237395199312</v>
       </c>
       <c r="G3" s="4">
-        <v>2.9279753968443697E-4</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="4">
-        <v>19.763689122637199</v>
-      </c>
-      <c r="J3" s="4">
-        <v>2.483241139549E-4</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" s="4">
-        <v>21.5770494047526</v>
-      </c>
-      <c r="M3" s="4">
-        <v>2.10294935854568E-5</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3" s="4">
-        <v>3.8623532293126499</v>
-      </c>
-      <c r="P3" s="4">
-        <v>5.7132906292297697E-2</v>
+        <v>7.07027773964158E-4</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>21.147760982538401</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3">
+        <v>51.4151226736616</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1</v>
+      </c>
+      <c r="O3" s="3">
+        <v>3.45065688668172</v>
+      </c>
+      <c r="P3" s="5">
+        <v>7.1421343791735606E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1.18694766411424E-2</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.91384944121357004</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1.10000951507023</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.30125445137128398</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4">
-        <v>1.4181998517729</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0.24764252610956899</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4" s="4">
-        <v>113.804564131031</v>
-      </c>
-      <c r="M4" s="4">
-        <v>4.1674708884916503E-15</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4" s="4">
-        <v>9.7244709217943398E-2</v>
-      </c>
-      <c r="P4" s="4">
-        <v>0.75696043995184303</v>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.18694766411464E-2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.91384944121355605</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1.1000095150704301</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.30125445137124102</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1.41819985177287</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.24764252610957299</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3">
+        <v>113.804564131078</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3">
+        <v>9.7244709217879699E-2</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0.75696043995191997</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>6.8357706683642702E-2</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.79523320122453001</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="4">
-        <v>3.0218002883814399</v>
-      </c>
-      <c r="G5" s="4">
-        <v>9.0699818525649206E-2</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0.467852370292895</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0.50182596240097299</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5" s="4">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>6.83577066836452E-2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.79523320122452701</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3.0218002883814301</v>
+      </c>
+      <c r="G5" s="5">
+        <v>9.0699818525649303E-2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.467852370292894</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.50182596240097399</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3">
         <v>108.085425093246</v>
       </c>
-      <c r="M5" s="4">
-        <v>1.0966392463473E-14</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5" s="4">
-        <v>6.5933298460407901</v>
+      <c r="M5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="3">
+        <v>6.5933298460407803</v>
       </c>
       <c r="P5" s="4">
         <v>1.4533845522818001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
-      <c r="B6">
+      <c r="B6" s="6">
         <v>36</v>
       </c>
-      <c r="E6">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6">
         <v>36</v>
       </c>
-      <c r="H6">
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6">
         <v>20</v>
       </c>
-      <c r="K6">
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6">
         <v>56</v>
       </c>
-      <c r="N6">
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
mods based on jeffs last comments. to do: - fix neightbor distance data - last check of doc
</commit_message>
<xml_diff>
--- a/analyses/tables/allometry.xlsx
+++ b/analyses/tables/allometry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicksmith/Documents/Git/mdi_pitchpine/analyses/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CFA90F-81DA-5149-9BC3-9A43D0D1C628}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7100EF-15BB-854E-8982-942CA213FAD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10960" yWindow="6160" windowWidth="26440" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10920" yWindow="6160" windowWidth="26440" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allometry" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>Elevation</t>
   </si>
@@ -29,18 +29,6 @@
   </si>
   <si>
     <t>Elevation:Fire</t>
-  </si>
-  <si>
-    <t>Canopy Spread (m)</t>
-  </si>
-  <si>
-    <t>DBH (cm)</t>
-  </si>
-  <si>
-    <t>Distance Between Neighbors (m)</t>
-  </si>
-  <si>
-    <t>Slope</t>
   </si>
   <si>
     <t>Df</t>
@@ -57,6 +45,15 @@
   <si>
     <t>&lt;0.001</t>
   </si>
+  <si>
+    <t>Canopy Spread</t>
+  </si>
+  <si>
+    <t>DBH</t>
+  </si>
+  <si>
+    <t>Distance Between Neighbors</t>
+  </si>
 </sst>
 </file>
 
@@ -207,18 +204,19 @@
       <family val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -566,10 +564,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -925,283 +929,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:P6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13" ht="14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>7.9478606241921899</v>
-      </c>
-      <c r="D3" s="4">
-        <v>7.7771897558913403E-3</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3">
-        <v>13.7237395199312</v>
-      </c>
-      <c r="G3" s="4">
-        <v>7.07027773964158E-4</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3">
-        <v>21.147760982538401</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="2">
-        <v>1</v>
-      </c>
-      <c r="L3" s="3">
-        <v>51.4151226736616</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3" s="2">
-        <v>1</v>
-      </c>
-      <c r="O3" s="3">
-        <v>3.45065688668172</v>
-      </c>
-      <c r="P3" s="5">
-        <v>7.1421343791735606E-2</v>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>12.6570657432339</v>
+      </c>
+      <c r="D3" s="6">
+        <v>7.7026288719703098E-4</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5">
+        <v>19.035051227968101</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5">
+        <v>10.0483124105168</v>
+      </c>
+      <c r="J3" s="6">
+        <v>2.4723598480186201E-3</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="5">
+        <v>13.1152720362625</v>
+      </c>
+      <c r="M3" s="6">
+        <v>6.3146642378540403E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" ht="14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.18694766411464E-2</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.91384944121355605</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1.1000095150704301</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.30125445137124102</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3">
-        <v>1.41819985177287</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.24764252610957299</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1</v>
-      </c>
-      <c r="L4" s="3">
-        <v>113.804564131078</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N4" s="2">
-        <v>1</v>
-      </c>
-      <c r="O4" s="3">
-        <v>9.7244709217879699E-2</v>
-      </c>
-      <c r="P4" s="3">
-        <v>0.75696043995191997</v>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>6.2621422747593299E-3</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.93720838352109104</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.55970837488775704</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.45750827930377502</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0.15476390664733999</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.69551754716309699</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.29583731520464501</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0.58866293199618303</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" ht="14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>6.83577066836452E-2</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.79523320122452701</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3">
-        <v>3.0218002883814301</v>
-      </c>
-      <c r="G5" s="5">
-        <v>9.0699818525649303E-2</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0.467852370292894</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0.50182596240097399</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
-      <c r="L5" s="3">
-        <v>108.085425093246</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N5" s="2">
-        <v>1</v>
-      </c>
-      <c r="O5" s="3">
-        <v>6.5933298460407803</v>
-      </c>
-      <c r="P5" s="4">
-        <v>1.4533845522818001E-2</v>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1.89018321256755</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.174657512964453</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>5.7741395493552599</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1.96018369419893E-2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0.96922667385679695</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.32910766574823902</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+      <c r="L5" s="5">
+        <v>14.8779127974693</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" ht="14" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="6">
-        <v>36</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6">
-        <v>36</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6">
-        <v>20</v>
-      </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6">
+      <c r="B6" s="3">
         <v>56</v>
       </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6">
-        <v>36</v>
-      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>56</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3">
+        <v>56</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3">
+        <v>56</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1212,8 +1170,6 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>